<commit_message>
Changes in Fragments.xlsx: - Added references to as many fragments as I know through out the forms
Changes in PreCalculation_NO.xdp:
- Changed references to the fragments
- Removed fields in TakstId row and replaced with Fragments/frg_IdDonebyDateSalemanInformation.xdp

Changes in ValuationReport_NO.xdp:
- Added correct references to new fragment names
- Removed fields in TakstId row and replaced with Fragments/frg_IdDonebyDateSalemanInformation.xdp

Changes in frg_TestLabel:
- Added try catch on all code for handling testlabels (otherwise there is an issue on production)

Added frg_IdDonebyDateSalesmanInformation

Signed-off-by: kcdc <kc@dafolo.dk>
</commit_message>
<xml_diff>
--- a/Dokumentation/Fragments.xlsx
+++ b/Dokumentation/Fragments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="36">
   <si>
     <t>CarPriceEstimate_NO</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>AcceptanceCheck_NO</t>
+  </si>
+  <si>
+    <t>frg_IdDonebyDateSalemanInformation</t>
   </si>
 </sst>
 </file>
@@ -511,16 +517,16 @@
   <dimension ref="A5:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
     <col min="2" max="16" width="4.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:16" ht="117" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="119.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -551,7 +557,9 @@
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -667,7 +675,9 @@
       <c r="J9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -725,7 +735,9 @@
       <c r="J11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -877,7 +889,9 @@
       <c r="J17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
@@ -911,7 +925,9 @@
       <c r="J18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
@@ -945,7 +961,9 @@
       <c r="J19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
@@ -983,7 +1001,9 @@
       <c r="J20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
@@ -1079,7 +1099,9 @@
       <c r="J23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
@@ -1111,7 +1133,9 @@
       <c r="J24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -1169,7 +1193,9 @@
       <c r="J26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -1207,7 +1233,9 @@
       <c r="J27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
@@ -1231,7 +1259,9 @@
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
@@ -1239,17 +1269,25 @@
       <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="K29" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>

</xml_diff>

<commit_message>
Changed in Fragments.xlsx: - Added references to fragments
Changed in Confirmation_NO.xdp:
- References to fragments

Changed in frg_LangNO.xdp
- Nothing but reinserted the same variables

Changed in frg_OverflowTrailer.xdp
- Removed Fragment references to languages

Changed in frg_ScriptGetLanguages.xdp
- Nothing, just reinserted the same code

Changed in Invoice_NO.xdp:
- added correct fragment references

Changed in PriceEstimate_NO.xdp:
- added fragment references

Changes in WorkOrder_BA.xdp:
- added correct references to fragments

Signed-off-by: kcdc <kc@dafolo.dk>
</commit_message>
<xml_diff>
--- a/Dokumentation/Fragments.xlsx
+++ b/Dokumentation/Fragments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="36">
   <si>
     <t>CarPriceEstimate_NO</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A5:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,10 +631,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1147,10 +1153,14 @@
         <v>29</v>
       </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>

</xml_diff>

<commit_message>
Fragments.xlsx: - removed frg_LogoHolder.xdp
No longer needed

Signed-off-by: kcdc <kc@dafolo.dk>
</commit_message>
<xml_diff>
--- a/Dokumentation/Fragments.xlsx
+++ b/Dokumentation/Fragments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="35">
   <si>
     <t>CarPriceEstimate_NO</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>frg_Logo</t>
-  </si>
-  <si>
-    <t>frg_LogoHolder</t>
   </si>
   <si>
     <t>frg_Metadata</t>
@@ -514,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:P34"/>
+  <dimension ref="A5:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +555,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -571,23 +568,23 @@
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -601,23 +598,23 @@
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -632,14 +629,14 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -657,32 +654,32 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -702,10 +699,10 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -719,30 +716,30 @@
         <v>15</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -758,12 +755,12 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -786,7 +783,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -801,25 +798,25 @@
         <v>18</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -840,7 +837,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -862,7 +859,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -877,26 +874,26 @@
         <v>21</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -909,30 +906,30 @@
         <v>22</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -945,30 +942,34 @@
         <v>23</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="I19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -981,35 +982,27 @@
         <v>24</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
@@ -1021,25 +1014,19 @@
         <v>25</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1053,21 +1040,35 @@
         <v>26</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="J22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -1079,34 +1080,28 @@
         <v>27</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1118,30 +1113,20 @@
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -1152,20 +1137,36 @@
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -1177,34 +1178,34 @@
         <v>30</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -1216,35 +1217,21 @@
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -1254,23 +1241,23 @@
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -1279,25 +1266,17 @@
       <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
@@ -1375,24 +1354,6 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in Fragments.xlsx: - added references for new fragments
Changes in frg_PriceInformation.xdp

- Added the fragment for CPE and CSC

Changes in CarPriceEstimate_NO.xdp

- Added fragment frg_PriceInformation.xdp

Changes in CarSalesContract_NO.xdp:
- Fixed numerous issues with fragments and pagination

Changes in Requisition_NO.xdp

- Changed logic for pagination
- Changed dynamics for defects and comments
- Changed binding on frg_IdDoneBy

Changes in frg_OverflowTrailer
- Added margin

Signed-off-by: kcdc <kc@dafolo.dk>
</commit_message>
<xml_diff>
--- a/Dokumentation/Fragments.xlsx
+++ b/Dokumentation/Fragments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="39">
   <si>
     <t>CarPriceEstimate_NO</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>frg_IdDonebyDateSalemanInformation</t>
+  </si>
+  <si>
+    <t>frg_PriceInformation</t>
+  </si>
+  <si>
+    <t>CarSalesContract_NO</t>
+  </si>
+  <si>
+    <t>Requisition_NO</t>
+  </si>
+  <si>
+    <t>VehicleControl_NO</t>
   </si>
 </sst>
 </file>
@@ -513,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:P19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,9 +569,15 @@
       <c r="K5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="4"/>
     </row>
@@ -587,7 +605,9 @@
         <v>32</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -617,7 +637,9 @@
         <v>32</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -643,7 +665,9 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -681,8 +705,12 @@
       <c r="K9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -741,8 +769,12 @@
       <c r="K11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -819,7 +851,9 @@
         <v>32</v>
       </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="L14" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -895,8 +929,12 @@
       <c r="K17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="L17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -931,8 +969,12 @@
       <c r="K18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="L18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -971,8 +1013,12 @@
       <c r="K19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="L19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -1029,7 +1075,9 @@
         <v>32</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="L21" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -1069,8 +1117,12 @@
       <c r="K22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="L22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -1103,8 +1155,12 @@
       <c r="K23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -1167,8 +1223,12 @@
       <c r="K25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -1207,8 +1267,12 @@
       <c r="K26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="L26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -1234,7 +1298,9 @@
         <v>32</v>
       </c>
       <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="M27" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -1260,14 +1326,20 @@
         <v>32</v>
       </c>
       <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="M28" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1277,7 +1349,9 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="L29" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>

</xml_diff>

<commit_message>
Updates to almost everywhere in the forms.
</commit_message>
<xml_diff>
--- a/Dokumentation/Fragments.xlsx
+++ b/Dokumentation/Fragments.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="47">
   <si>
     <t>CarPriceEstimate_NO</t>
   </si>
@@ -625,7 +625,7 @@
   <dimension ref="A4:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,9 @@
       <c r="N8" s="8"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>

</xml_diff>